<commit_message>
Criação dos cadastros de status e local de tratamento
</commit_message>
<xml_diff>
--- a/script_base_dados/grants_solus.xlsx
+++ b/script_base_dados/grants_solus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\solus\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DEB83F-944B-4635-A9CC-6BBB46E7AD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF889181-6670-4D6F-9817-8C59D85BFCED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
   <sheets>
     <sheet name="grants" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="66">
   <si>
     <t>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO</t>
   </si>
@@ -215,13 +215,31 @@
   </si>
   <si>
     <t xml:space="preserve">GRANT SELECT ON  TABLE tratamento.vw_menu_princ_usua TO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_local_trtmto TO </t>
+  </si>
+  <si>
+    <t>GRANT SELECT ON SEQUENCE tratamento.sq_local_trtmto TO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_status_trtmto TO </t>
+  </si>
+  <si>
+    <t>GRANT SELECT ON SEQUENCE tratamento.sq_status_trtmto TO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_risco_pcnt TO </t>
+  </si>
+  <si>
+    <t>GRANT SELECT ON SEQUENCE tratamento.sq_risco_pcnt TO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,12 +252,6 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -262,12 +274,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3049,18 +3060,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F5A992-25FF-475C-9CF2-7DC64A66C30C}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D29"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="95.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="105" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="100.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3089,7 +3098,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D29" si="0">A2&amp;" "&amp;B2&amp;" "&amp;C2</f>
+        <f t="shared" ref="D2:D35" si="0">A2&amp;" "&amp;B2&amp;" "&amp;C2</f>
         <v>GRANT CONNECT ON DATABASE desenv TO  evaldo ;</v>
       </c>
     </row>
@@ -3498,8 +3507,95 @@
         <v>GRANT SELECT ON SEQUENCE tratamento.sq_pnel_solic_trtmto TO evaldo ;</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_local_trtmto TO  evaldo ;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT ON SEQUENCE tratamento.sq_local_trtmto TO evaldo ;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_status_trtmto TO  evaldo ;</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT ON SEQUENCE tratamento.sq_status_trtmto TO evaldo ;</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_risco_pcnt TO  evaldo ;</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT ON SEQUENCE tratamento.sq_risco_pcnt TO evaldo ;</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Atualização de banco de dados
</commit_message>
<xml_diff>
--- a/script_base_dados/grants_solus.xlsx
+++ b/script_base_dados/grants_solus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\solus\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF889181-6670-4D6F-9817-8C59D85BFCED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76D7BD9-73CA-4DA8-8293-4E28E6FE8B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
@@ -172,9 +172,6 @@
     <t xml:space="preserve">GRANT DELETE, UPDATE, INSERT, SELECT ON tratamento.tb_c_log_acesso TO </t>
   </si>
   <si>
-    <t>evaldo</t>
-  </si>
-  <si>
     <t xml:space="preserve">GRANT CONNECT ON DATABASE desenv TO </t>
   </si>
   <si>
@@ -233,6 +230,9 @@
   </si>
   <si>
     <t>GRANT SELECT ON SEQUENCE tratamento.sq_risco_pcnt TO</t>
+  </si>
+  <si>
+    <t>vanessa</t>
   </si>
 </sst>
 </file>
@@ -3062,44 +3062,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F5A992-25FF-475C-9CF2-7DC64A66C30C}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="95.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="100.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C1" t="s">
         <v>32</v>
       </c>
       <c r="D1" t="str">
         <f>A1&amp;" "&amp;B1&amp;" "&amp;C1</f>
-        <v>CREATE USER  evaldo PASSWORD '1234';</v>
+        <v>CREATE USER  vanessa PASSWORD '1234';</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D35" si="0">A2&amp;" "&amp;B2&amp;" "&amp;C2</f>
-        <v>GRANT CONNECT ON DATABASE desenv TO  evaldo ;</v>
+        <v>GRANT CONNECT ON DATABASE desenv TO  vanessa ;</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3107,14 +3109,14 @@
         <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT USAGE ON SCHEMA tratamento TO  evaldo ;</v>
+        <v>GRANT USAGE ON SCHEMA tratamento TO  vanessa ;</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3122,14 +3124,14 @@
         <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON ALL TABLES IN SCHEMA tratamento TO  evaldo ;</v>
+        <v>GRANT SELECT ON ALL TABLES IN SCHEMA tratamento TO  vanessa ;</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3137,14 +3139,14 @@
         <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA tratamento TO  evaldo ;</v>
+        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA tratamento TO  vanessa ;</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3152,14 +3154,14 @@
         <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on tratamento.vw_menu_princ_tratamento TO evaldo ;</v>
+        <v>GRANT SELECT on tratamento.vw_menu_princ_tratamento TO vanessa ;</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3167,14 +3169,14 @@
         <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on tratamento.vw_menu_princ_tratamento_usua TO  evaldo ;</v>
+        <v>GRANT SELECT on tratamento.vw_menu_princ_tratamento_usua TO  vanessa ;</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3182,14 +3184,14 @@
         <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on tratamento.vw_menu_princ_usua TO  evaldo ;</v>
+        <v>GRANT SELECT on tratamento.vw_menu_princ_usua TO  vanessa ;</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3197,14 +3199,14 @@
         <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_grupo_acesso TO  evaldo ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_grupo_acesso TO  vanessa ;</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3212,14 +3214,14 @@
         <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_grupo_usua_acesso TO  evaldo ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_grupo_usua_acesso TO  vanessa ;</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3227,14 +3229,14 @@
         <v>41</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_grupo_usua_menu_sist_tratamento TO  evaldo ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_grupo_usua_menu_sist_tratamento TO  vanessa ;</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3242,14 +3244,14 @@
         <v>42</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_menu_sist_tratamento TO  evaldo ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_menu_sist_tratamento TO  vanessa ;</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3257,14 +3259,14 @@
         <v>43</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_usua_acesso TO  evaldo ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_usua_acesso TO  vanessa ;</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3272,329 +3274,329 @@
         <v>44</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON tratamento.tb_c_log_acesso TO  evaldo ;</v>
+        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON tratamento.tb_c_log_acesso TO  vanessa ;</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_menu_princ_tratamento TO evaldo ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_menu_princ_tratamento TO vanessa ;</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
         <v>1</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_menu_princ_tratamento_usua TO evaldo ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_menu_princ_tratamento_usua TO vanessa ;</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_menu_princ_usua TO  evaldo ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_menu_princ_usua TO  vanessa ;</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
         <v>1</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON SEQUENCE tratamento.sq_log_acesso TO evaldo ;</v>
+        <v>GRANT SELECT ON SEQUENCE tratamento.sq_log_acesso TO vanessa ;</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON SEQUENCE tratamento.sq_acesso_transac_tratamento TO evaldo ;</v>
+        <v>GRANT SELECT ON SEQUENCE tratamento.sq_acesso_transac_tratamento TO vanessa ;</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON SEQUENCE tratamento.sq_grupo_usua_acesso TO evaldo ;</v>
+        <v>GRANT SELECT ON SEQUENCE tratamento.sq_grupo_usua_acesso TO vanessa ;</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON SEQUENCE tratamento.sq_grupo_usua_menu_sist_tratamento TO evaldo ;</v>
+        <v>GRANT SELECT ON SEQUENCE tratamento.sq_grupo_usua_menu_sist_tratamento TO vanessa ;</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C22" t="s">
         <v>1</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON SEQUENCE tratamento.sq_grupo_usua_transac_acesso TO evaldo ;</v>
+        <v>GRANT SELECT ON SEQUENCE tratamento.sq_grupo_usua_transac_acesso TO vanessa ;</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON SEQUENCE tratamento.sq_log_acesso TO evaldo ;</v>
+        <v>GRANT SELECT ON SEQUENCE tratamento.sq_log_acesso TO vanessa ;</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
         <v>1</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON SEQUENCE tratamento.sq_menu_sist_tratamento TO evaldo ;</v>
+        <v>GRANT SELECT ON SEQUENCE tratamento.sq_menu_sist_tratamento TO vanessa ;</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON SEQUENCE tratamento.sq_usua_acesso TO evaldo ;</v>
+        <v>GRANT SELECT ON SEQUENCE tratamento.sq_usua_acesso TO vanessa ;</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON SEQUENCE tratamento.sq_equipe TO evaldo ;</v>
+        <v>GRANT SELECT ON SEQUENCE tratamento.sq_equipe TO vanessa ;</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON SEQUENCE tratamento.sq_status_equipe TO evaldo ;</v>
+        <v>GRANT SELECT ON SEQUENCE tratamento.sq_status_equipe TO vanessa ;</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C28" t="s">
         <v>1</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON SEQUENCE tratamento.sq_status_equipe TO evaldo ;</v>
+        <v>GRANT SELECT ON SEQUENCE tratamento.sq_status_equipe TO vanessa ;</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C29" t="s">
         <v>1</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON SEQUENCE tratamento.sq_pnel_solic_trtmto TO evaldo ;</v>
+        <v>GRANT SELECT ON SEQUENCE tratamento.sq_pnel_solic_trtmto TO vanessa ;</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_local_trtmto TO  evaldo ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_local_trtmto TO  vanessa ;</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C31" t="s">
         <v>1</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON SEQUENCE tratamento.sq_local_trtmto TO evaldo ;</v>
+        <v>GRANT SELECT ON SEQUENCE tratamento.sq_local_trtmto TO vanessa ;</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C32" t="s">
         <v>1</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_status_trtmto TO  evaldo ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_status_trtmto TO  vanessa ;</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C33" t="s">
         <v>1</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON SEQUENCE tratamento.sq_status_trtmto TO evaldo ;</v>
+        <v>GRANT SELECT ON SEQUENCE tratamento.sq_status_trtmto TO vanessa ;</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C34" t="s">
         <v>1</v>
       </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_risco_pcnt TO  evaldo ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_risco_pcnt TO  vanessa ;</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C35" t="s">
         <v>1</v>
       </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON SEQUENCE tratamento.sq_risco_pcnt TO evaldo ;</v>
+        <v>GRANT SELECT ON SEQUENCE tratamento.sq_risco_pcnt TO vanessa ;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Criação da base de dados para o painel de tratamento
</commit_message>
<xml_diff>
--- a/script_base_dados/grants_solus.xlsx
+++ b/script_base_dados/grants_solus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\solus\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76D7BD9-73CA-4DA8-8293-4E28E6FE8B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46F3A58-4A79-4AD2-9B65-30B7072A07DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
   <sheets>
     <sheet name="grants" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="68">
   <si>
     <t>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO</t>
   </si>
@@ -233,6 +233,12 @@
   </si>
   <si>
     <t>vanessa</t>
+  </si>
+  <si>
+    <t>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_obs_pnel_solic_trtmto TO</t>
+  </si>
+  <si>
+    <t>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_pnel_solic_trtmto TO</t>
   </si>
 </sst>
 </file>
@@ -3060,11 +3066,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F5A992-25FF-475C-9CF2-7DC64A66C30C}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3100,7 +3104,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D35" si="0">A2&amp;" "&amp;B2&amp;" "&amp;C2</f>
+        <f t="shared" ref="D2:D37" si="0">A2&amp;" "&amp;B2&amp;" "&amp;C2</f>
         <v>GRANT CONNECT ON DATABASE desenv TO  vanessa ;</v>
       </c>
     </row>
@@ -3597,6 +3601,36 @@
       <c r="D35" t="str">
         <f t="shared" si="0"/>
         <v>GRANT SELECT ON SEQUENCE tratamento.sq_risco_pcnt TO vanessa ;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_obs_pnel_solic_trtmto TO vanessa ;</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_pnel_solic_trtmto TO vanessa ;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Status do tratamento e acompanhamentotratamento.php
</commit_message>
<xml_diff>
--- a/script_base_dados/grants_solus.xlsx
+++ b/script_base_dados/grants_solus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\solus\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A03523-BB20-4FAE-83F2-1350FE3EC226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C028D917-7006-44CB-81DC-F0BE3AA24826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="70">
   <si>
     <t>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO</t>
   </si>
@@ -242,6 +242,9 @@
   </si>
   <si>
     <t xml:space="preserve">GRANT ALL ON SEQUENCE tratamento.sq_grupo_acesso TO </t>
+  </si>
+  <si>
+    <t>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_mncp to</t>
   </si>
 </sst>
 </file>
@@ -3069,10 +3072,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F5A992-25FF-475C-9CF2-7DC64A66C30C}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3109,7 +3112,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D37" si="0">A2&amp;" "&amp;B2&amp;" "&amp;C2</f>
+        <f t="shared" ref="D2:D38" si="0">A2&amp;" "&amp;B2&amp;" "&amp;C2</f>
         <v>GRANT CONNECT ON DATABASE solus TO  aline ;</v>
       </c>
     </row>
@@ -3636,6 +3639,21 @@
       <c r="D37" t="str">
         <f t="shared" si="0"/>
         <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_acesso TO  aline ;</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_mncp to aline ;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Criação da tela de acompanhamentotratamento.php
</commit_message>
<xml_diff>
--- a/script_base_dados/grants_solus.xlsx
+++ b/script_base_dados/grants_solus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\solus\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C028D917-7006-44CB-81DC-F0BE3AA24826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0384CC39-4D53-4002-BB4F-D74B45C85AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="73">
   <si>
     <t>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO</t>
   </si>
@@ -245,6 +245,15 @@
   </si>
   <si>
     <t>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_mncp to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT ALL ON SEQUENCE tratamento.sq_hstr_pnel_solic_trtmto TO </t>
+  </si>
+  <si>
+    <t>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_pcnt TO</t>
+  </si>
+  <si>
+    <t>GRANT SELECT ON  TABLE tratamento.vw_painel_trtmto TO</t>
   </si>
 </sst>
 </file>
@@ -3072,10 +3081,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F5A992-25FF-475C-9CF2-7DC64A66C30C}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3112,7 +3121,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D38" si="0">A2&amp;" "&amp;B2&amp;" "&amp;C2</f>
+        <f t="shared" ref="D2:D42" si="0">A2&amp;" "&amp;B2&amp;" "&amp;C2</f>
         <v>GRANT CONNECT ON DATABASE solus TO  aline ;</v>
       </c>
     </row>
@@ -3654,6 +3663,66 @@
       <c r="D38" t="str">
         <f t="shared" si="0"/>
         <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_mncp to aline ;</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_pnel_solic_trtmto TO aline ;</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_pnel_solic_trtmto TO  aline ;</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_pcnt TO aline ;</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_painel_trtmto TO aline ;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
acompanhamentotratamento.php. Inclusão de status e cálculo do tempo de status.
</commit_message>
<xml_diff>
--- a/script_base_dados/grants_solus.xlsx
+++ b/script_base_dados/grants_solus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\solus\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0384CC39-4D53-4002-BB4F-D74B45C85AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F24CB6-AD4B-4C4D-94CF-C04D74775A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="74">
   <si>
     <t>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO</t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t>GRANT SELECT ON  TABLE tratamento.vw_painel_trtmto TO</t>
+  </si>
+  <si>
+    <t>GRANT ALL ON SEQUENCE tratamento.sq_hstr_obs_pnel_solic_trtmto TO</t>
   </si>
 </sst>
 </file>
@@ -3081,11 +3084,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F5A992-25FF-475C-9CF2-7DC64A66C30C}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3121,7 +3122,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D42" si="0">A2&amp;" "&amp;B2&amp;" "&amp;C2</f>
+        <f t="shared" ref="D2:D43" si="0">A2&amp;" "&amp;B2&amp;" "&amp;C2</f>
         <v>GRANT CONNECT ON DATABASE solus TO  aline ;</v>
       </c>
     </row>
@@ -3723,6 +3724,21 @@
       <c r="D42" t="str">
         <f t="shared" si="0"/>
         <v>GRANT SELECT ON  TABLE tratamento.vw_painel_trtmto TO aline ;</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_obs_pnel_solic_trtmto TO aline ;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alterações para implatação do mapa de tratamento
</commit_message>
<xml_diff>
--- a/script_base_dados/grants_solus.xlsx
+++ b/script_base_dados/grants_solus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\solus\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F24CB6-AD4B-4C4D-94CF-C04D74775A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1373839A-EA96-4280-9170-7C487E8E3426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="81">
   <si>
     <t>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO</t>
   </si>
@@ -238,9 +238,6 @@
     <t xml:space="preserve">GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_status_pcnt TO </t>
   </si>
   <si>
-    <t>aline</t>
-  </si>
-  <si>
     <t xml:space="preserve">GRANT ALL ON SEQUENCE tratamento.sq_grupo_acesso TO </t>
   </si>
   <si>
@@ -257,6 +254,30 @@
   </si>
   <si>
     <t>GRANT ALL ON SEQUENCE tratamento.sq_hstr_obs_pnel_solic_trtmto TO</t>
+  </si>
+  <si>
+    <t>GRANT ALL ON SEQUENCE tratamento.sq_risco_rnado_pcnt TO</t>
+  </si>
+  <si>
+    <t>GRANT ALL ON SEQUENCE tratamento.sq_hstr_pnel_mapa_risco TO</t>
+  </si>
+  <si>
+    <t>GRANT ALL ON SEQUENCE tratamento.sq_hstr_obs_pnel_mapa_risco TO</t>
+  </si>
+  <si>
+    <t>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_obs_pnel_mapa_risco TO</t>
+  </si>
+  <si>
+    <t>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_pnel_mapa_risco TO</t>
+  </si>
+  <si>
+    <t>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_risco_rnado_pcnt TO</t>
+  </si>
+  <si>
+    <t>vanessa</t>
+  </si>
+  <si>
+    <t>evaldo</t>
   </si>
 </sst>
 </file>
@@ -3084,7 +3105,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F5A992-25FF-475C-9CF2-7DC64A66C30C}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3101,14 +3122,14 @@
         <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
         <v>32</v>
       </c>
       <c r="D1" t="str">
         <f>A1&amp;" "&amp;B1&amp;" "&amp;C1</f>
-        <v>CREATE USER  aline PASSWORD '1234';</v>
+        <v>CREATE USER  vanessa PASSWORD '1234';</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3116,14 +3137,14 @@
         <v>64</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D43" si="0">A2&amp;" "&amp;B2&amp;" "&amp;C2</f>
-        <v>GRANT CONNECT ON DATABASE solus TO  aline ;</v>
+        <f t="shared" ref="D2:D49" si="0">A2&amp;" "&amp;B2&amp;" "&amp;C2</f>
+        <v>GRANT CONNECT ON DATABASE solus TO  vanessa ;</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3131,14 +3152,14 @@
         <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT USAGE ON SCHEMA tratamento TO  aline ;</v>
+        <v>GRANT USAGE ON SCHEMA tratamento TO  vanessa ;</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3146,14 +3167,14 @@
         <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON ALL TABLES IN SCHEMA tratamento TO  aline ;</v>
+        <v>GRANT SELECT ON ALL TABLES IN SCHEMA tratamento TO  vanessa ;</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3161,14 +3182,14 @@
         <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA tratamento TO  aline ;</v>
+        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA tratamento TO  vanessa ;</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3176,14 +3197,14 @@
         <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on tratamento.vw_menu_princ_tratamento TO aline ;</v>
+        <v>GRANT SELECT on tratamento.vw_menu_princ_tratamento TO vanessa ;</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3191,14 +3212,14 @@
         <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on tratamento.vw_menu_princ_tratamento_usua TO  aline ;</v>
+        <v>GRANT SELECT on tratamento.vw_menu_princ_tratamento_usua TO  vanessa ;</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3206,14 +3227,14 @@
         <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on tratamento.vw_menu_princ_usua TO  aline ;</v>
+        <v>GRANT SELECT on tratamento.vw_menu_princ_usua TO  vanessa ;</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3221,14 +3242,14 @@
         <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_grupo_acesso TO  aline ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_grupo_acesso TO  vanessa ;</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3236,14 +3257,14 @@
         <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_grupo_usua_acesso TO  aline ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_grupo_usua_acesso TO  vanessa ;</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3251,14 +3272,14 @@
         <v>41</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_grupo_usua_menu_sist_tratamento TO  aline ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_grupo_usua_menu_sist_tratamento TO  vanessa ;</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3266,14 +3287,14 @@
         <v>42</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_menu_sist_tratamento TO  aline ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_menu_sist_tratamento TO  vanessa ;</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3281,14 +3302,14 @@
         <v>43</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_usua_acesso TO  aline ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_usua_acesso TO  vanessa ;</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3296,14 +3317,14 @@
         <v>44</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON tratamento.tb_c_log_acesso TO  aline ;</v>
+        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON tratamento.tb_c_log_acesso TO  vanessa ;</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3311,14 +3332,14 @@
         <v>45</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_menu_princ_tratamento TO aline ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_menu_princ_tratamento TO vanessa ;</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3326,14 +3347,14 @@
         <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s">
         <v>1</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_menu_princ_tratamento_usua TO aline ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_menu_princ_tratamento_usua TO vanessa ;</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3341,14 +3362,14 @@
         <v>47</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_menu_princ_usua TO  aline ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_menu_princ_usua TO  vanessa ;</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3356,14 +3377,14 @@
         <v>54</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
         <v>1</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_log_acesso TO aline ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_log_acesso TO vanessa ;</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3371,14 +3392,14 @@
         <v>55</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_acesso_transac_tratamento TO aline ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_acesso_transac_tratamento TO vanessa ;</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3386,14 +3407,14 @@
         <v>56</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_usua_acesso TO aline ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_usua_acesso TO vanessa ;</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3401,14 +3422,14 @@
         <v>57</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_usua_menu_sist_tratamento TO aline ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_usua_menu_sist_tratamento TO vanessa ;</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3416,14 +3437,14 @@
         <v>58</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
         <v>1</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_usua_transac_acesso TO aline ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_usua_transac_acesso TO vanessa ;</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3431,14 +3452,14 @@
         <v>54</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_log_acesso TO aline ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_log_acesso TO vanessa ;</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3446,14 +3467,14 @@
         <v>59</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C24" t="s">
         <v>1</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_menu_sist_tratamento TO aline ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_menu_sist_tratamento TO vanessa ;</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3461,14 +3482,14 @@
         <v>60</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_usua_acesso TO aline ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_usua_acesso TO vanessa ;</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3476,14 +3497,14 @@
         <v>61</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe TO aline ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe TO vanessa ;</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3491,14 +3512,14 @@
         <v>62</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_status_equipe TO aline ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_status_equipe TO vanessa ;</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3506,14 +3527,14 @@
         <v>63</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C28" t="s">
         <v>1</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_pnel_solic_trtmto TO aline ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pnel_solic_trtmto TO vanessa ;</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3521,14 +3542,14 @@
         <v>48</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C29" t="s">
         <v>1</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_local_trtmto TO  aline ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_local_trtmto TO  vanessa ;</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3536,14 +3557,14 @@
         <v>49</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON SEQUENCE tratamento.sq_local_trtmto TO aline ;</v>
+        <v>GRANT SELECT ON SEQUENCE tratamento.sq_local_trtmto TO vanessa ;</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3551,14 +3572,14 @@
         <v>66</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C31" t="s">
         <v>1</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_status_pcnt TO  aline ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_status_pcnt TO  vanessa ;</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3566,14 +3587,14 @@
         <v>65</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C32" t="s">
         <v>1</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON SEQUENCE tratamento.sq_status_pcnt TO aline ;</v>
+        <v>GRANT SELECT ON SEQUENCE tratamento.sq_status_pcnt TO vanessa ;</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3581,14 +3602,14 @@
         <v>50</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C33" t="s">
         <v>1</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_risco_pcnt TO  aline ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_risco_pcnt TO  vanessa ;</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3596,14 +3617,14 @@
         <v>51</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C34" t="s">
         <v>1</v>
       </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON SEQUENCE tratamento.sq_risco_pcnt TO aline ;</v>
+        <v>GRANT SELECT ON SEQUENCE tratamento.sq_risco_pcnt TO vanessa ;</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3611,14 +3632,14 @@
         <v>52</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
       </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_obs_pnel_solic_trtmto TO aline ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_obs_pnel_solic_trtmto TO vanessa ;</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3626,44 +3647,44 @@
         <v>53</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C36" t="s">
         <v>1</v>
       </c>
       <c r="D36" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_pnel_solic_trtmto TO aline ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_pnel_solic_trtmto TO vanessa ;</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C37" t="s">
         <v>1</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_acesso TO  aline ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_acesso TO  vanessa ;</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C38" t="s">
         <v>1</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_mncp to aline ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_mncp to vanessa ;</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3671,74 +3692,164 @@
         <v>53</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C39" t="s">
         <v>1</v>
       </c>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_pnel_solic_trtmto TO aline ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_pnel_solic_trtmto TO vanessa ;</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C40" t="s">
         <v>1</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_pnel_solic_trtmto TO  aline ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_pnel_solic_trtmto TO  vanessa ;</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C41" t="s">
         <v>1</v>
       </c>
       <c r="D41" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_pcnt TO aline ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_pcnt TO vanessa ;</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C42" t="s">
         <v>1</v>
       </c>
       <c r="D42" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_painel_trtmto TO aline ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_painel_trtmto TO vanessa ;</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_obs_pnel_solic_trtmto TO evaldo ;</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>73</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C43" t="s">
-        <v>1</v>
-      </c>
-      <c r="D43" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_obs_pnel_solic_trtmto TO aline ;</v>
+      <c r="B44" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_risco_rnado_pcnt TO evaldo ;</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_pnel_mapa_risco TO evaldo ;</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_obs_pnel_mapa_risco TO evaldo ;</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_obs_pnel_mapa_risco TO evaldo ;</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_pnel_mapa_risco TO evaldo ;</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>78</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_risco_rnado_pcnt TO evaldo ;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cadastro de transações e relatório de acompanhamentotratamento.php
</commit_message>
<xml_diff>
--- a/script_base_dados/grants_solus.xlsx
+++ b/script_base_dados/grants_solus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\solus\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1373839A-EA96-4280-9170-7C487E8E3426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E7D4AB-5F74-48E9-925B-1EA73E661489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="92">
   <si>
     <t>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO</t>
   </si>
@@ -223,18 +223,12 @@
     <t>GRANT ALL ON SEQUENCE tratamento.sq_equipe TO</t>
   </si>
   <si>
-    <t>GRANT ALL ON SEQUENCE tratamento.sq_status_equipe TO</t>
-  </si>
-  <si>
     <t>GRANT ALL ON SEQUENCE tratamento.sq_pnel_solic_trtmto TO</t>
   </si>
   <si>
     <t xml:space="preserve">GRANT CONNECT ON DATABASE solus TO </t>
   </si>
   <si>
-    <t>GRANT SELECT ON SEQUENCE tratamento.sq_status_pcnt TO</t>
-  </si>
-  <si>
     <t xml:space="preserve">GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_status_pcnt TO </t>
   </si>
   <si>
@@ -274,10 +268,49 @@
     <t>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_risco_rnado_pcnt TO</t>
   </si>
   <si>
-    <t>vanessa</t>
-  </si>
-  <si>
-    <t>evaldo</t>
+    <t>"marcia.costa"</t>
+  </si>
+  <si>
+    <t>"mariana.brider"</t>
+  </si>
+  <si>
+    <t>"adriana.paes"</t>
+  </si>
+  <si>
+    <t>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO</t>
+  </si>
+  <si>
+    <t>"kleverson.antonio"</t>
+  </si>
+  <si>
+    <t>"luana.mourao"</t>
+  </si>
+  <si>
+    <t>"larissa.rocha"</t>
+  </si>
+  <si>
+    <t>"livia.hallack"</t>
+  </si>
+  <si>
+    <t>"vanessa.cirilo"</t>
+  </si>
+  <si>
+    <t>"milena.ribeiral"</t>
+  </si>
+  <si>
+    <t>"tatiane.neto"</t>
+  </si>
+  <si>
+    <t>"tatyene.nehrer"</t>
+  </si>
+  <si>
+    <t>"victor.quinet"</t>
+  </si>
+  <si>
+    <t>"lidice.lenz"</t>
+  </si>
+  <si>
+    <t>"alberlania.muller"</t>
   </si>
 </sst>
 </file>
@@ -3105,14 +3138,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F5A992-25FF-475C-9CF2-7DC64A66C30C}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="95.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="100.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -3129,12 +3164,12 @@
       </c>
       <c r="D1" t="str">
         <f>A1&amp;" "&amp;B1&amp;" "&amp;C1</f>
-        <v>CREATE USER  vanessa PASSWORD '1234';</v>
+        <v>CREATE USER  "adriana.paes" PASSWORD '1234';</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>79</v>
@@ -3143,8 +3178,8 @@
         <v>1</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D49" si="0">A2&amp;" "&amp;B2&amp;" "&amp;C2</f>
-        <v>GRANT CONNECT ON DATABASE solus TO  vanessa ;</v>
+        <f t="shared" ref="D2:D61" si="0">A2&amp;" "&amp;B2&amp;" "&amp;C2</f>
+        <v>GRANT CONNECT ON DATABASE solus TO  "adriana.paes" ;</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3159,7 +3194,7 @@
       </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT USAGE ON SCHEMA tratamento TO  vanessa ;</v>
+        <v>GRANT USAGE ON SCHEMA tratamento TO  "adriana.paes" ;</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3174,7 +3209,7 @@
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON ALL TABLES IN SCHEMA tratamento TO  vanessa ;</v>
+        <v>GRANT SELECT ON ALL TABLES IN SCHEMA tratamento TO  "adriana.paes" ;</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3189,7 +3224,7 @@
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA tratamento TO  vanessa ;</v>
+        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA tratamento TO  "adriana.paes" ;</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3204,7 +3239,7 @@
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on tratamento.vw_menu_princ_tratamento TO vanessa ;</v>
+        <v>GRANT SELECT on tratamento.vw_menu_princ_tratamento TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3219,7 +3254,7 @@
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on tratamento.vw_menu_princ_tratamento_usua TO  vanessa ;</v>
+        <v>GRANT SELECT on tratamento.vw_menu_princ_tratamento_usua TO  "adriana.paes" ;</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3234,7 +3269,7 @@
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on tratamento.vw_menu_princ_usua TO  vanessa ;</v>
+        <v>GRANT SELECT on tratamento.vw_menu_princ_usua TO  "adriana.paes" ;</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3249,7 +3284,7 @@
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_grupo_acesso TO  vanessa ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_grupo_acesso TO  "adriana.paes" ;</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3264,7 +3299,7 @@
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_grupo_usua_acesso TO  vanessa ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_grupo_usua_acesso TO  "adriana.paes" ;</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3279,7 +3314,7 @@
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_grupo_usua_menu_sist_tratamento TO  vanessa ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_grupo_usua_menu_sist_tratamento TO  "adriana.paes" ;</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3294,7 +3329,7 @@
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_menu_sist_tratamento TO  vanessa ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_menu_sist_tratamento TO  "adriana.paes" ;</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3309,7 +3344,7 @@
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_usua_acesso TO  vanessa ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_usua_acesso TO  "adriana.paes" ;</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3324,7 +3359,7 @@
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON tratamento.tb_c_log_acesso TO  vanessa ;</v>
+        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON tratamento.tb_c_log_acesso TO  "adriana.paes" ;</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3339,7 +3374,7 @@
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_menu_princ_tratamento TO vanessa ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_menu_princ_tratamento TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3354,7 +3389,7 @@
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_menu_princ_tratamento_usua TO vanessa ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_menu_princ_tratamento_usua TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3369,7 +3404,7 @@
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_menu_princ_usua TO  vanessa ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_menu_princ_usua TO  "adriana.paes" ;</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3384,7 +3419,7 @@
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_log_acesso TO vanessa ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_log_acesso TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3399,7 +3434,7 @@
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_acesso_transac_tratamento TO vanessa ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_acesso_transac_tratamento TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3414,7 +3449,7 @@
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_usua_acesso TO vanessa ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_usua_acesso TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3429,7 +3464,7 @@
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_usua_menu_sist_tratamento TO vanessa ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_usua_menu_sist_tratamento TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3444,7 +3479,7 @@
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_usua_transac_acesso TO vanessa ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_usua_transac_acesso TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3459,7 +3494,7 @@
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_log_acesso TO vanessa ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_log_acesso TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3474,7 +3509,7 @@
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_menu_sist_tratamento TO vanessa ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_menu_sist_tratamento TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3489,7 +3524,7 @@
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_usua_acesso TO vanessa ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_usua_acesso TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3504,7 +3539,7 @@
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe TO vanessa ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3519,12 +3554,12 @@
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_status_equipe TO vanessa ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pnel_solic_trtmto TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>79</v>
@@ -3534,12 +3569,12 @@
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_pnel_solic_trtmto TO vanessa ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_local_trtmto TO  "adriana.paes" ;</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>79</v>
@@ -3549,12 +3584,12 @@
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_local_trtmto TO  vanessa ;</v>
+        <v>GRANT SELECT ON SEQUENCE tratamento.sq_local_trtmto TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>79</v>
@@ -3564,12 +3599,12 @@
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON SEQUENCE tratamento.sq_local_trtmto TO vanessa ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_status_pcnt TO  "adriana.paes" ;</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>79</v>
@@ -3579,12 +3614,12 @@
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_status_pcnt TO  vanessa ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_risco_pcnt TO  "adriana.paes" ;</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>79</v>
@@ -3594,12 +3629,12 @@
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON SEQUENCE tratamento.sq_status_pcnt TO vanessa ;</v>
+        <v>GRANT SELECT ON SEQUENCE tratamento.sq_risco_pcnt TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>79</v>
@@ -3609,12 +3644,12 @@
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_risco_pcnt TO  vanessa ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_obs_pnel_solic_trtmto TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>79</v>
@@ -3624,12 +3659,12 @@
       </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON SEQUENCE tratamento.sq_risco_pcnt TO vanessa ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_pnel_solic_trtmto TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>79</v>
@@ -3639,12 +3674,12 @@
       </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_obs_pnel_solic_trtmto TO vanessa ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_acesso TO  "adriana.paes" ;</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>79</v>
@@ -3654,12 +3689,12 @@
       </c>
       <c r="D36" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_pnel_solic_trtmto TO vanessa ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_mncp to "adriana.paes" ;</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>79</v>
@@ -3669,12 +3704,12 @@
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_acesso TO  vanessa ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_pnel_solic_trtmto TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>79</v>
@@ -3684,12 +3719,12 @@
       </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_mncp to vanessa ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_pnel_solic_trtmto TO  "adriana.paes" ;</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>79</v>
@@ -3699,7 +3734,7 @@
       </c>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_pnel_solic_trtmto TO vanessa ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_pcnt TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3714,7 +3749,7 @@
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_pnel_solic_trtmto TO  vanessa ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_painel_trtmto TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3729,7 +3764,7 @@
       </c>
       <c r="D41" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_pcnt TO vanessa ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_obs_pnel_solic_trtmto TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3744,7 +3779,7 @@
       </c>
       <c r="D42" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_painel_trtmto TO vanessa ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_risco_rnado_pcnt TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3752,14 +3787,14 @@
         <v>72</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C43" t="s">
         <v>1</v>
       </c>
       <c r="D43" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_obs_pnel_solic_trtmto TO evaldo ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_pnel_mapa_risco TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3767,14 +3802,14 @@
         <v>73</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C44" t="s">
         <v>1</v>
       </c>
       <c r="D44" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_risco_rnado_pcnt TO evaldo ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_obs_pnel_mapa_risco TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3782,14 +3817,14 @@
         <v>74</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C45" t="s">
         <v>1</v>
       </c>
       <c r="D45" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_pnel_mapa_risco TO evaldo ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_obs_pnel_mapa_risco TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3797,14 +3832,14 @@
         <v>75</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C46" t="s">
         <v>1</v>
       </c>
       <c r="D46" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_obs_pnel_mapa_risco TO evaldo ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_pnel_mapa_risco TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -3812,44 +3847,224 @@
         <v>76</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C47" t="s">
         <v>1</v>
       </c>
       <c r="D47" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_obs_pnel_mapa_risco TO evaldo ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_risco_rnado_pcnt TO "adriana.paes" ;</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C48" t="s">
         <v>1</v>
       </c>
       <c r="D48" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_pnel_mapa_risco TO evaldo ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "kleverson.antonio" ;</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "luana.mourao" ;</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>80</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C50" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>80</v>
       </c>
-      <c r="C49" t="s">
-        <v>1</v>
-      </c>
-      <c r="D49" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_risco_rnado_pcnt TO evaldo ;</v>
+      <c r="B51" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "adriana.paes" ;</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>80</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "larissa.rocha" ;</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>80</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "livia.hallack" ;</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>80</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "vanessa.cirilo" ;</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>80</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "milena.ribeiral" ;</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>80</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "tatiane.neto" ;</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>80</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "tatyene.nehrer" ;</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>80</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C58" t="s">
+        <v>1</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "victor.quinet" ;</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>80</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "lidice.lenz" ;</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>80</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C60" t="s">
+        <v>1</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "alberlania.muller" ;</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>80</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "marcia.costa" ;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Manutenção do pedido de tratamento
</commit_message>
<xml_diff>
--- a/script_base_dados/grants_solus.xlsx
+++ b/script_base_dados/grants_solus.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\solus\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E7D4AB-5F74-48E9-925B-1EA73E661489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD1CCED-6F7E-4274-A9D4-032A740F6976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="97">
   <si>
     <t>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO</t>
   </si>
@@ -311,6 +311,21 @@
   </si>
   <si>
     <t>"alberlania.muller"</t>
+  </si>
+  <si>
+    <t>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO</t>
+  </si>
+  <si>
+    <t>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO</t>
+  </si>
+  <si>
+    <t>vanessa</t>
+  </si>
+  <si>
+    <t>aline</t>
+  </si>
+  <si>
+    <t>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO</t>
   </si>
 </sst>
 </file>
@@ -3138,10 +3153,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F5A992-25FF-475C-9CF2-7DC64A66C30C}">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="B88" workbookViewId="0">
+      <selection activeCell="D95" sqref="D95:D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3178,7 +3193,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D61" si="0">A2&amp;" "&amp;B2&amp;" "&amp;C2</f>
+        <f t="shared" ref="D2:D65" si="0">A2&amp;" "&amp;B2&amp;" "&amp;C2</f>
         <v>GRANT CONNECT ON DATABASE solus TO  "adriana.paes" ;</v>
       </c>
     </row>
@@ -4065,6 +4080,771 @@
       <c r="D61" t="str">
         <f t="shared" si="0"/>
         <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "marcia.costa" ;</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>92</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "adriana.paes" ;</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>92</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "kleverson.antonio" ;</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>92</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "luana.mourao" ;</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>92</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>92</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" ref="D66:D112" si="1">A66&amp;" "&amp;B66&amp;" "&amp;C66</f>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "adriana.paes" ;</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>92</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "larissa.rocha" ;</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>92</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "livia.hallack" ;</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>92</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C69" t="s">
+        <v>1</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "vanessa.cirilo" ;</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>92</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "milena.ribeiral" ;</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>92</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "tatiane.neto" ;</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>92</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C72" t="s">
+        <v>1</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "tatyene.nehrer" ;</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>92</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C73" t="s">
+        <v>1</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "victor.quinet" ;</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>92</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "lidice.lenz" ;</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>92</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C75" t="s">
+        <v>1</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "alberlania.muller" ;</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>92</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C76" t="s">
+        <v>1</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "marcia.costa" ;</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>92</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C77" t="s">
+        <v>1</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO vanessa ;</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>92</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C78" t="s">
+        <v>1</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO aline ;</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>93</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C79" t="s">
+        <v>1</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "adriana.paes" ;</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>93</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C80" t="s">
+        <v>1</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "kleverson.antonio" ;</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>93</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C81" t="s">
+        <v>1</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "luana.mourao" ;</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>93</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C82" t="s">
+        <v>1</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>93</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C83" t="s">
+        <v>1</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "adriana.paes" ;</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>93</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1</v>
+      </c>
+      <c r="D84" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "larissa.rocha" ;</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>93</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C85" t="s">
+        <v>1</v>
+      </c>
+      <c r="D85" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "livia.hallack" ;</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>93</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1</v>
+      </c>
+      <c r="D86" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "vanessa.cirilo" ;</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>93</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1</v>
+      </c>
+      <c r="D87" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "milena.ribeiral" ;</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>93</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C88" t="s">
+        <v>1</v>
+      </c>
+      <c r="D88" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "tatiane.neto" ;</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>93</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C89" t="s">
+        <v>1</v>
+      </c>
+      <c r="D89" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "tatyene.nehrer" ;</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>93</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C90" t="s">
+        <v>1</v>
+      </c>
+      <c r="D90" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "victor.quinet" ;</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>93</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C91" t="s">
+        <v>1</v>
+      </c>
+      <c r="D91" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "lidice.lenz" ;</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>93</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C92" t="s">
+        <v>1</v>
+      </c>
+      <c r="D92" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "alberlania.muller" ;</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>93</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C93" t="s">
+        <v>1</v>
+      </c>
+      <c r="D93" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "marcia.costa" ;</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>93</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C94" t="s">
+        <v>1</v>
+      </c>
+      <c r="D94" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO vanessa ;</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>93</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C95" t="s">
+        <v>1</v>
+      </c>
+      <c r="D95" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO aline ;</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>96</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C96" t="s">
+        <v>1</v>
+      </c>
+      <c r="D96" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "adriana.paes" ;</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>96</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C97" t="s">
+        <v>1</v>
+      </c>
+      <c r="D97" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "kleverson.antonio" ;</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>96</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C98" t="s">
+        <v>1</v>
+      </c>
+      <c r="D98" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "luana.mourao" ;</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>96</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C99" t="s">
+        <v>1</v>
+      </c>
+      <c r="D99" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>96</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C100" t="s">
+        <v>1</v>
+      </c>
+      <c r="D100" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "adriana.paes" ;</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>96</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C101" t="s">
+        <v>1</v>
+      </c>
+      <c r="D101" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "larissa.rocha" ;</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>96</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C102" t="s">
+        <v>1</v>
+      </c>
+      <c r="D102" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "livia.hallack" ;</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>96</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C103" t="s">
+        <v>1</v>
+      </c>
+      <c r="D103" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "vanessa.cirilo" ;</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>96</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C104" t="s">
+        <v>1</v>
+      </c>
+      <c r="D104" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "milena.ribeiral" ;</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>96</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C105" t="s">
+        <v>1</v>
+      </c>
+      <c r="D105" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "tatiane.neto" ;</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>96</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C106" t="s">
+        <v>1</v>
+      </c>
+      <c r="D106" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "tatyene.nehrer" ;</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>96</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C107" t="s">
+        <v>1</v>
+      </c>
+      <c r="D107" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "victor.quinet" ;</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>96</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C108" t="s">
+        <v>1</v>
+      </c>
+      <c r="D108" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "lidice.lenz" ;</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>96</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C109" t="s">
+        <v>1</v>
+      </c>
+      <c r="D109" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "alberlania.muller" ;</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>96</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C110" t="s">
+        <v>1</v>
+      </c>
+      <c r="D110" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "marcia.costa" ;</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>96</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C111" t="s">
+        <v>1</v>
+      </c>
+      <c r="D111" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO vanessa ;</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>96</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C112" t="s">
+        <v>1</v>
+      </c>
+      <c r="D112" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO aline ;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cadastro da relação Usuário X Equipe
</commit_message>
<xml_diff>
--- a/script_base_dados/grants_solus.xlsx
+++ b/script_base_dados/grants_solus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\solus\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D71770-3C27-4F94-8FC8-91C0EA9E1204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43C81EB-82F9-43CD-9E79-97F3465B84AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="101">
   <si>
     <t>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO</t>
   </si>
@@ -332,6 +332,12 @@
   </si>
   <si>
     <t>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO</t>
+  </si>
+  <si>
+    <t>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO</t>
+  </si>
+  <si>
+    <t>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO</t>
   </si>
 </sst>
 </file>
@@ -3159,11 +3165,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F5A992-25FF-475C-9CF2-7DC64A66C30C}">
-  <dimension ref="A1:D148"/>
+  <dimension ref="A1:D184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="D131" sqref="D131:D148"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5119,7 +5123,7 @@
         <v>1</v>
       </c>
       <c r="D130" t="str">
-        <f t="shared" ref="D130:D148" si="2">A130&amp;" "&amp;B130&amp;" "&amp;C130</f>
+        <f t="shared" ref="D130:D184" si="2">A130&amp;" "&amp;B130&amp;" "&amp;C130</f>
         <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO aline ;</v>
       </c>
     </row>
@@ -5391,6 +5395,546 @@
       <c r="D148" t="str">
         <f t="shared" si="2"/>
         <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO aline ;</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>99</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C149" t="s">
+        <v>1</v>
+      </c>
+      <c r="D149" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO aline ;</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>99</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C150" t="s">
+        <v>1</v>
+      </c>
+      <c r="D150" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "adriana.paes" ;</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>99</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C151" t="s">
+        <v>1</v>
+      </c>
+      <c r="D151" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "kleverson.antonio" ;</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>99</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C152" t="s">
+        <v>1</v>
+      </c>
+      <c r="D152" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "luana.mourao" ;</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>99</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C153" t="s">
+        <v>1</v>
+      </c>
+      <c r="D153" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>99</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C154" t="s">
+        <v>1</v>
+      </c>
+      <c r="D154" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "adriana.paes" ;</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>99</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C155" t="s">
+        <v>1</v>
+      </c>
+      <c r="D155" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "larissa.rocha" ;</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>99</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C156" t="s">
+        <v>1</v>
+      </c>
+      <c r="D156" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "livia.hallack" ;</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>99</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C157" t="s">
+        <v>1</v>
+      </c>
+      <c r="D157" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "vanessa.cirilo" ;</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>99</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C158" t="s">
+        <v>1</v>
+      </c>
+      <c r="D158" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "milena.ribeiral" ;</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>99</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C159" t="s">
+        <v>1</v>
+      </c>
+      <c r="D159" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "tatiane.neto" ;</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>99</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C160" t="s">
+        <v>1</v>
+      </c>
+      <c r="D160" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "tatyene.nehrer" ;</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>99</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C161" t="s">
+        <v>1</v>
+      </c>
+      <c r="D161" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "victor.quinet" ;</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>99</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C162" t="s">
+        <v>1</v>
+      </c>
+      <c r="D162" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "lidice.lenz" ;</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>99</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C163" t="s">
+        <v>1</v>
+      </c>
+      <c r="D163" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "alberlania.muller" ;</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>99</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C164" t="s">
+        <v>1</v>
+      </c>
+      <c r="D164" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "marcia.costa" ;</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>99</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C165" t="s">
+        <v>1</v>
+      </c>
+      <c r="D165" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO vanessa ;</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>99</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C166" t="s">
+        <v>1</v>
+      </c>
+      <c r="D166" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO aline ;</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>100</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C167" t="s">
+        <v>1</v>
+      </c>
+      <c r="D167" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO aline ;</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>100</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C168" t="s">
+        <v>1</v>
+      </c>
+      <c r="D168" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "adriana.paes" ;</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>100</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C169" t="s">
+        <v>1</v>
+      </c>
+      <c r="D169" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "kleverson.antonio" ;</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>100</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C170" t="s">
+        <v>1</v>
+      </c>
+      <c r="D170" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "luana.mourao" ;</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>100</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C171" t="s">
+        <v>1</v>
+      </c>
+      <c r="D171" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>100</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C172" t="s">
+        <v>1</v>
+      </c>
+      <c r="D172" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "adriana.paes" ;</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>100</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C173" t="s">
+        <v>1</v>
+      </c>
+      <c r="D173" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "larissa.rocha" ;</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>100</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C174" t="s">
+        <v>1</v>
+      </c>
+      <c r="D174" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "livia.hallack" ;</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>100</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C175" t="s">
+        <v>1</v>
+      </c>
+      <c r="D175" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "vanessa.cirilo" ;</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>100</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C176" t="s">
+        <v>1</v>
+      </c>
+      <c r="D176" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "milena.ribeiral" ;</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>100</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C177" t="s">
+        <v>1</v>
+      </c>
+      <c r="D177" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "tatiane.neto" ;</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>100</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C178" t="s">
+        <v>1</v>
+      </c>
+      <c r="D178" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "tatyene.nehrer" ;</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>100</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C179" t="s">
+        <v>1</v>
+      </c>
+      <c r="D179" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "victor.quinet" ;</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>100</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C180" t="s">
+        <v>1</v>
+      </c>
+      <c r="D180" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "lidice.lenz" ;</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>100</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C181" t="s">
+        <v>1</v>
+      </c>
+      <c r="D181" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "alberlania.muller" ;</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>100</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C182" t="s">
+        <v>1</v>
+      </c>
+      <c r="D182" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "marcia.costa" ;</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>100</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C183" t="s">
+        <v>1</v>
+      </c>
+      <c r="D183" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO vanessa ;</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>100</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C184" t="s">
+        <v>1</v>
+      </c>
+      <c r="D184" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO aline ;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Letras maiúsculas para o status de tratamento
</commit_message>
<xml_diff>
--- a/script_base_dados/grants_solus.xlsx
+++ b/script_base_dados/grants_solus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\solus\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43C81EB-82F9-43CD-9E79-97F3465B84AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57956E22-DAF9-45F7-9C94-4C5B8937B0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="86">
   <si>
     <t>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO</t>
   </si>
@@ -268,63 +268,15 @@
     <t>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_risco_rnado_pcnt TO</t>
   </si>
   <si>
-    <t>"marcia.costa"</t>
-  </si>
-  <si>
-    <t>"mariana.brider"</t>
-  </si>
-  <si>
-    <t>"adriana.paes"</t>
-  </si>
-  <si>
     <t>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO</t>
   </si>
   <si>
-    <t>"kleverson.antonio"</t>
-  </si>
-  <si>
-    <t>"luana.mourao"</t>
-  </si>
-  <si>
-    <t>"larissa.rocha"</t>
-  </si>
-  <si>
-    <t>"livia.hallack"</t>
-  </si>
-  <si>
-    <t>"vanessa.cirilo"</t>
-  </si>
-  <si>
-    <t>"milena.ribeiral"</t>
-  </si>
-  <si>
-    <t>"tatiane.neto"</t>
-  </si>
-  <si>
-    <t>"tatyene.nehrer"</t>
-  </si>
-  <si>
-    <t>"victor.quinet"</t>
-  </si>
-  <si>
-    <t>"lidice.lenz"</t>
-  </si>
-  <si>
-    <t>"alberlania.muller"</t>
-  </si>
-  <si>
     <t>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO</t>
   </si>
   <si>
     <t>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO</t>
   </si>
   <si>
-    <t>vanessa</t>
-  </si>
-  <si>
-    <t>aline</t>
-  </si>
-  <si>
     <t>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO</t>
   </si>
   <si>
@@ -338,6 +290,9 @@
   </si>
   <si>
     <t>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO</t>
+  </si>
+  <si>
+    <t>"alice.gomes"</t>
   </si>
 </sst>
 </file>
@@ -3182,14 +3137,14 @@
         <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C1" t="s">
         <v>32</v>
       </c>
       <c r="D1" t="str">
         <f>A1&amp;" "&amp;B1&amp;" "&amp;C1</f>
-        <v>CREATE USER  "adriana.paes" PASSWORD '1234';</v>
+        <v>CREATE USER  "alice.gomes" PASSWORD '1234';</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3197,14 +3152,14 @@
         <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D65" si="0">A2&amp;" "&amp;B2&amp;" "&amp;C2</f>
-        <v>GRANT CONNECT ON DATABASE solus TO  "adriana.paes" ;</v>
+        <v>GRANT CONNECT ON DATABASE solus TO  "alice.gomes" ;</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3212,14 +3167,14 @@
         <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT USAGE ON SCHEMA tratamento TO  "adriana.paes" ;</v>
+        <v>GRANT USAGE ON SCHEMA tratamento TO  "alice.gomes" ;</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3227,14 +3182,14 @@
         <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON ALL TABLES IN SCHEMA tratamento TO  "adriana.paes" ;</v>
+        <v>GRANT SELECT ON ALL TABLES IN SCHEMA tratamento TO  "alice.gomes" ;</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3242,14 +3197,14 @@
         <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA tratamento TO  "adriana.paes" ;</v>
+        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA tratamento TO  "alice.gomes" ;</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3257,14 +3212,14 @@
         <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on tratamento.vw_menu_princ_tratamento TO "adriana.paes" ;</v>
+        <v>GRANT SELECT on tratamento.vw_menu_princ_tratamento TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3272,14 +3227,14 @@
         <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on tratamento.vw_menu_princ_tratamento_usua TO  "adriana.paes" ;</v>
+        <v>GRANT SELECT on tratamento.vw_menu_princ_tratamento_usua TO  "alice.gomes" ;</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3287,14 +3242,14 @@
         <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on tratamento.vw_menu_princ_usua TO  "adriana.paes" ;</v>
+        <v>GRANT SELECT on tratamento.vw_menu_princ_usua TO  "alice.gomes" ;</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3302,14 +3257,14 @@
         <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_grupo_acesso TO  "adriana.paes" ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_grupo_acesso TO  "alice.gomes" ;</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3317,14 +3272,14 @@
         <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_grupo_usua_acesso TO  "adriana.paes" ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_grupo_usua_acesso TO  "alice.gomes" ;</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3332,14 +3287,14 @@
         <v>41</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_grupo_usua_menu_sist_tratamento TO  "adriana.paes" ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_grupo_usua_menu_sist_tratamento TO  "alice.gomes" ;</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3347,14 +3302,14 @@
         <v>42</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_menu_sist_tratamento TO  "adriana.paes" ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_menu_sist_tratamento TO  "alice.gomes" ;</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3362,14 +3317,14 @@
         <v>43</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_usua_acesso TO  "adriana.paes" ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_usua_acesso TO  "alice.gomes" ;</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3377,14 +3332,14 @@
         <v>44</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON tratamento.tb_c_log_acesso TO  "adriana.paes" ;</v>
+        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON tratamento.tb_c_log_acesso TO  "alice.gomes" ;</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3392,14 +3347,14 @@
         <v>45</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_menu_princ_tratamento TO "adriana.paes" ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_menu_princ_tratamento TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3407,14 +3362,14 @@
         <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C16" t="s">
         <v>1</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_menu_princ_tratamento_usua TO "adriana.paes" ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_menu_princ_tratamento_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3422,14 +3377,14 @@
         <v>47</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_menu_princ_usua TO  "adriana.paes" ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_menu_princ_usua TO  "alice.gomes" ;</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3437,14 +3392,14 @@
         <v>54</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C18" t="s">
         <v>1</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_log_acesso TO "adriana.paes" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_log_acesso TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3452,14 +3407,14 @@
         <v>55</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_acesso_transac_tratamento TO "adriana.paes" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_acesso_transac_tratamento TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3467,14 +3422,14 @@
         <v>56</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_usua_acesso TO "adriana.paes" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_usua_acesso TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3482,14 +3437,14 @@
         <v>57</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_usua_menu_sist_tratamento TO "adriana.paes" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_usua_menu_sist_tratamento TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3497,14 +3452,14 @@
         <v>58</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C22" t="s">
         <v>1</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_usua_transac_acesso TO "adriana.paes" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_usua_transac_acesso TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3512,14 +3467,14 @@
         <v>54</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_log_acesso TO "adriana.paes" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_log_acesso TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3527,14 +3482,14 @@
         <v>59</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C24" t="s">
         <v>1</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_menu_sist_tratamento TO "adriana.paes" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_menu_sist_tratamento TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3542,14 +3497,14 @@
         <v>60</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_usua_acesso TO "adriana.paes" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_usua_acesso TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3557,14 +3512,14 @@
         <v>61</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe TO "adriana.paes" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3572,14 +3527,14 @@
         <v>62</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_pnel_solic_trtmto TO "adriana.paes" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pnel_solic_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3587,14 +3542,14 @@
         <v>48</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C28" t="s">
         <v>1</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_local_trtmto TO  "adriana.paes" ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_local_trtmto TO  "alice.gomes" ;</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3602,14 +3557,14 @@
         <v>49</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C29" t="s">
         <v>1</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON SEQUENCE tratamento.sq_local_trtmto TO "adriana.paes" ;</v>
+        <v>GRANT SELECT ON SEQUENCE tratamento.sq_local_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3617,14 +3572,14 @@
         <v>64</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_status_pcnt TO  "adriana.paes" ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_status_pcnt TO  "alice.gomes" ;</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3632,14 +3587,14 @@
         <v>50</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C31" t="s">
         <v>1</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_risco_pcnt TO  "adriana.paes" ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON tratamento.tb_c_risco_pcnt TO  "alice.gomes" ;</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3647,14 +3602,14 @@
         <v>51</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C32" t="s">
         <v>1</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON SEQUENCE tratamento.sq_risco_pcnt TO "adriana.paes" ;</v>
+        <v>GRANT SELECT ON SEQUENCE tratamento.sq_risco_pcnt TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3662,14 +3617,14 @@
         <v>52</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C33" t="s">
         <v>1</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_obs_pnel_solic_trtmto TO "adriana.paes" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_obs_pnel_solic_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3677,14 +3632,14 @@
         <v>53</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C34" t="s">
         <v>1</v>
       </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_pnel_solic_trtmto TO "adriana.paes" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_pnel_solic_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3692,14 +3647,14 @@
         <v>65</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
       </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_acesso TO  "adriana.paes" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_acesso TO  "alice.gomes" ;</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3707,14 +3662,14 @@
         <v>66</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C36" t="s">
         <v>1</v>
       </c>
       <c r="D36" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_mncp to "adriana.paes" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_mncp to "alice.gomes" ;</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -3722,14 +3677,14 @@
         <v>53</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C37" t="s">
         <v>1</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_pnel_solic_trtmto TO "adriana.paes" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_pnel_solic_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -3737,14 +3692,14 @@
         <v>67</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C38" t="s">
         <v>1</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_pnel_solic_trtmto TO  "adriana.paes" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_pnel_solic_trtmto TO  "alice.gomes" ;</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3752,14 +3707,14 @@
         <v>68</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C39" t="s">
         <v>1</v>
       </c>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_pcnt TO "adriana.paes" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_pcnt TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3767,14 +3722,14 @@
         <v>69</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C40" t="s">
         <v>1</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_painel_trtmto TO "adriana.paes" ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_painel_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3782,14 +3737,14 @@
         <v>70</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C41" t="s">
         <v>1</v>
       </c>
       <c r="D41" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_obs_pnel_solic_trtmto TO "adriana.paes" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_obs_pnel_solic_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3797,14 +3752,14 @@
         <v>71</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C42" t="s">
         <v>1</v>
       </c>
       <c r="D42" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_risco_rnado_pcnt TO "adriana.paes" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_risco_rnado_pcnt TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3812,14 +3767,14 @@
         <v>72</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C43" t="s">
         <v>1</v>
       </c>
       <c r="D43" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_pnel_mapa_risco TO "adriana.paes" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_pnel_mapa_risco TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3827,14 +3782,14 @@
         <v>73</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C44" t="s">
         <v>1</v>
       </c>
       <c r="D44" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_obs_pnel_mapa_risco TO "adriana.paes" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_obs_pnel_mapa_risco TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3842,14 +3797,14 @@
         <v>74</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C45" t="s">
         <v>1</v>
       </c>
       <c r="D45" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_obs_pnel_mapa_risco TO "adriana.paes" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_obs_pnel_mapa_risco TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3857,14 +3812,14 @@
         <v>75</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C46" t="s">
         <v>1</v>
       </c>
       <c r="D46" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_pnel_mapa_risco TO "adriana.paes" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_hstr_pnel_mapa_risco TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -3872,109 +3827,109 @@
         <v>76</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C47" t="s">
         <v>1</v>
       </c>
       <c r="D47" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_risco_rnado_pcnt TO "adriana.paes" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_risco_rnado_pcnt TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C48" t="s">
         <v>1</v>
       </c>
       <c r="D48" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "kleverson.antonio" ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C49" t="s">
         <v>1</v>
       </c>
       <c r="D49" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "luana.mourao" ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C50" t="s">
         <v>1</v>
       </c>
       <c r="D50" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "mariana.brider" ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C51" t="s">
         <v>1</v>
       </c>
       <c r="D51" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "adriana.paes" ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C52" t="s">
         <v>1</v>
       </c>
       <c r="D52" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "larissa.rocha" ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C53" t="s">
         <v>1</v>
       </c>
       <c r="D53" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "livia.hallack" ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>85</v>
@@ -3984,222 +3939,222 @@
       </c>
       <c r="D54" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "vanessa.cirilo" ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C55" t="s">
         <v>1</v>
       </c>
       <c r="D55" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "milena.ribeiral" ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C56" t="s">
         <v>1</v>
       </c>
       <c r="D56" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "tatiane.neto" ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C57" t="s">
         <v>1</v>
       </c>
       <c r="D57" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "tatyene.nehrer" ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C58" t="s">
         <v>1</v>
       </c>
       <c r="D58" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "victor.quinet" ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C59" t="s">
         <v>1</v>
       </c>
       <c r="D59" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "lidice.lenz" ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C60" t="s">
         <v>1</v>
       </c>
       <c r="D60" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "alberlania.muller" ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C61" t="s">
         <v>1</v>
       </c>
       <c r="D61" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "marcia.costa" ;</v>
+        <v>GRANT SELECT ON  TABLE tratamento.vw_acesso_transac_tratamento TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C62" t="s">
         <v>1</v>
       </c>
       <c r="D62" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "adriana.paes" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C63" t="s">
         <v>1</v>
       </c>
       <c r="D63" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "kleverson.antonio" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C64" t="s">
         <v>1</v>
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "luana.mourao" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C65" t="s">
         <v>1</v>
       </c>
       <c r="D65" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "mariana.brider" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C66" t="s">
         <v>1</v>
       </c>
       <c r="D66" t="str">
         <f t="shared" ref="D66:D129" si="1">A66&amp;" "&amp;B66&amp;" "&amp;C66</f>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "adriana.paes" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C67" t="s">
         <v>1</v>
       </c>
       <c r="D67" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "larissa.rocha" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C68" t="s">
         <v>1</v>
       </c>
       <c r="D68" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "livia.hallack" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>85</v>
@@ -4209,252 +4164,252 @@
       </c>
       <c r="D69" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "vanessa.cirilo" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C70" t="s">
         <v>1</v>
       </c>
       <c r="D70" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "milena.ribeiral" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C71" t="s">
         <v>1</v>
       </c>
       <c r="D71" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "tatiane.neto" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C72" t="s">
         <v>1</v>
       </c>
       <c r="D72" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "tatyene.nehrer" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C73" t="s">
         <v>1</v>
       </c>
       <c r="D73" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "victor.quinet" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C74" t="s">
         <v>1</v>
       </c>
       <c r="D74" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "lidice.lenz" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C75" t="s">
         <v>1</v>
       </c>
       <c r="D75" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "alberlania.muller" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C76" t="s">
         <v>1</v>
       </c>
       <c r="D76" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "marcia.costa" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C77" t="s">
         <v>1</v>
       </c>
       <c r="D77" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO vanessa ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C78" t="s">
         <v>1</v>
       </c>
       <c r="D78" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO aline ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C79" t="s">
         <v>1</v>
       </c>
       <c r="D79" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "adriana.paes" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C80" t="s">
         <v>1</v>
       </c>
       <c r="D80" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "kleverson.antonio" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C81" t="s">
         <v>1</v>
       </c>
       <c r="D81" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "luana.mourao" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C82" t="s">
         <v>1</v>
       </c>
       <c r="D82" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "mariana.brider" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C83" t="s">
         <v>1</v>
       </c>
       <c r="D83" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "adriana.paes" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C84" t="s">
         <v>1</v>
       </c>
       <c r="D84" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "larissa.rocha" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C85" t="s">
         <v>1</v>
       </c>
       <c r="D85" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "livia.hallack" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>85</v>
@@ -4464,252 +4419,252 @@
       </c>
       <c r="D86" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "vanessa.cirilo" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C87" t="s">
         <v>1</v>
       </c>
       <c r="D87" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "milena.ribeiral" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C88" t="s">
         <v>1</v>
       </c>
       <c r="D88" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "tatiane.neto" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C89" t="s">
         <v>1</v>
       </c>
       <c r="D89" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "tatyene.nehrer" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C90" t="s">
         <v>1</v>
       </c>
       <c r="D90" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "victor.quinet" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C91" t="s">
         <v>1</v>
       </c>
       <c r="D91" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "lidice.lenz" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C92" t="s">
         <v>1</v>
       </c>
       <c r="D92" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "alberlania.muller" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C93" t="s">
         <v>1</v>
       </c>
       <c r="D93" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "marcia.costa" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C94" t="s">
         <v>1</v>
       </c>
       <c r="D94" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO vanessa ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C95" t="s">
         <v>1</v>
       </c>
       <c r="D95" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO aline ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C96" t="s">
         <v>1</v>
       </c>
       <c r="D96" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "adriana.paes" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C97" t="s">
         <v>1</v>
       </c>
       <c r="D97" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "kleverson.antonio" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C98" t="s">
         <v>1</v>
       </c>
       <c r="D98" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "luana.mourao" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C99" t="s">
         <v>1</v>
       </c>
       <c r="D99" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "mariana.brider" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C100" t="s">
         <v>1</v>
       </c>
       <c r="D100" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "adriana.paes" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C101" t="s">
         <v>1</v>
       </c>
       <c r="D101" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "larissa.rocha" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C102" t="s">
         <v>1</v>
       </c>
       <c r="D102" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "livia.hallack" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>85</v>
@@ -4719,267 +4674,267 @@
       </c>
       <c r="D103" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "vanessa.cirilo" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C104" t="s">
         <v>1</v>
       </c>
       <c r="D104" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "milena.ribeiral" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C105" t="s">
         <v>1</v>
       </c>
       <c r="D105" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "tatiane.neto" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C106" t="s">
         <v>1</v>
       </c>
       <c r="D106" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "tatyene.nehrer" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C107" t="s">
         <v>1</v>
       </c>
       <c r="D107" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "victor.quinet" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C108" t="s">
         <v>1</v>
       </c>
       <c r="D108" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "lidice.lenz" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C109" t="s">
         <v>1</v>
       </c>
       <c r="D109" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "alberlania.muller" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C110" t="s">
         <v>1</v>
       </c>
       <c r="D110" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "marcia.costa" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C111" t="s">
         <v>1</v>
       </c>
       <c r="D111" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO vanessa ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C112" t="s">
         <v>1</v>
       </c>
       <c r="D112" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO aline ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cid TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C113" t="s">
         <v>1</v>
       </c>
       <c r="D113" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO aline ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C114" t="s">
         <v>1</v>
       </c>
       <c r="D114" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "adriana.paes" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C115" t="s">
         <v>1</v>
       </c>
       <c r="D115" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "kleverson.antonio" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C116" t="s">
         <v>1</v>
       </c>
       <c r="D116" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "luana.mourao" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C117" t="s">
         <v>1</v>
       </c>
       <c r="D117" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "mariana.brider" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C118" t="s">
         <v>1</v>
       </c>
       <c r="D118" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "adriana.paes" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C119" t="s">
         <v>1</v>
       </c>
       <c r="D119" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "larissa.rocha" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C120" t="s">
         <v>1</v>
       </c>
       <c r="D120" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "livia.hallack" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>85</v>
@@ -4989,267 +4944,267 @@
       </c>
       <c r="D121" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "vanessa.cirilo" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C122" t="s">
         <v>1</v>
       </c>
       <c r="D122" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "milena.ribeiral" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C123" t="s">
         <v>1</v>
       </c>
       <c r="D123" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "tatiane.neto" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C124" t="s">
         <v>1</v>
       </c>
       <c r="D124" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "tatyene.nehrer" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C125" t="s">
         <v>1</v>
       </c>
       <c r="D125" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "victor.quinet" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C126" t="s">
         <v>1</v>
       </c>
       <c r="D126" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "lidice.lenz" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C127" t="s">
         <v>1</v>
       </c>
       <c r="D127" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "alberlania.muller" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C128" t="s">
         <v>1</v>
       </c>
       <c r="D128" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "marcia.costa" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C129" t="s">
         <v>1</v>
       </c>
       <c r="D129" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO vanessa ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C130" t="s">
         <v>1</v>
       </c>
       <c r="D130" t="str">
         <f t="shared" ref="D130:D184" si="2">A130&amp;" "&amp;B130&amp;" "&amp;C130</f>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO aline ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C131" t="s">
         <v>1</v>
       </c>
       <c r="D131" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO aline ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C132" t="s">
         <v>1</v>
       </c>
       <c r="D132" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "adriana.paes" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C133" t="s">
         <v>1</v>
       </c>
       <c r="D133" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "kleverson.antonio" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C134" t="s">
         <v>1</v>
       </c>
       <c r="D134" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "luana.mourao" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C135" t="s">
         <v>1</v>
       </c>
       <c r="D135" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "mariana.brider" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C136" t="s">
         <v>1</v>
       </c>
       <c r="D136" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "adriana.paes" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C137" t="s">
         <v>1</v>
       </c>
       <c r="D137" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "larissa.rocha" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C138" t="s">
         <v>1</v>
       </c>
       <c r="D138" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "livia.hallack" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>85</v>
@@ -5259,267 +5214,267 @@
       </c>
       <c r="D139" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "vanessa.cirilo" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C140" t="s">
         <v>1</v>
       </c>
       <c r="D140" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "milena.ribeiral" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C141" t="s">
         <v>1</v>
       </c>
       <c r="D141" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "tatiane.neto" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C142" t="s">
         <v>1</v>
       </c>
       <c r="D142" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "tatyene.nehrer" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C143" t="s">
         <v>1</v>
       </c>
       <c r="D143" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "victor.quinet" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C144" t="s">
         <v>1</v>
       </c>
       <c r="D144" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "lidice.lenz" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C145" t="s">
         <v>1</v>
       </c>
       <c r="D145" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "alberlania.muller" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C146" t="s">
         <v>1</v>
       </c>
       <c r="D146" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "marcia.costa" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C147" t="s">
         <v>1</v>
       </c>
       <c r="D147" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO vanessa ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C148" t="s">
         <v>1</v>
       </c>
       <c r="D148" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO aline ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C149" t="s">
         <v>1</v>
       </c>
       <c r="D149" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO aline ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C150" t="s">
         <v>1</v>
       </c>
       <c r="D150" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "adriana.paes" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C151" t="s">
         <v>1</v>
       </c>
       <c r="D151" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "kleverson.antonio" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C152" t="s">
         <v>1</v>
       </c>
       <c r="D152" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "luana.mourao" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C153" t="s">
         <v>1</v>
       </c>
       <c r="D153" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "mariana.brider" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C154" t="s">
         <v>1</v>
       </c>
       <c r="D154" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "adriana.paes" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C155" t="s">
         <v>1</v>
       </c>
       <c r="D155" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "larissa.rocha" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C156" t="s">
         <v>1</v>
       </c>
       <c r="D156" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "livia.hallack" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>85</v>
@@ -5529,267 +5484,267 @@
       </c>
       <c r="D157" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "vanessa.cirilo" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C158" t="s">
         <v>1</v>
       </c>
       <c r="D158" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "milena.ribeiral" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C159" t="s">
         <v>1</v>
       </c>
       <c r="D159" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "tatiane.neto" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C160" t="s">
         <v>1</v>
       </c>
       <c r="D160" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "tatyene.nehrer" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C161" t="s">
         <v>1</v>
       </c>
       <c r="D161" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "victor.quinet" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C162" t="s">
         <v>1</v>
       </c>
       <c r="D162" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "lidice.lenz" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C163" t="s">
         <v>1</v>
       </c>
       <c r="D163" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "alberlania.muller" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C164" t="s">
         <v>1</v>
       </c>
       <c r="D164" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "marcia.costa" ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C165" t="s">
         <v>1</v>
       </c>
       <c r="D165" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO vanessa ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C166" t="s">
         <v>1</v>
       </c>
       <c r="D166" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO aline ;</v>
+        <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C167" t="s">
         <v>1</v>
       </c>
       <c r="D167" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO aline ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C168" t="s">
         <v>1</v>
       </c>
       <c r="D168" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "adriana.paes" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C169" t="s">
         <v>1</v>
       </c>
       <c r="D169" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "kleverson.antonio" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C170" t="s">
         <v>1</v>
       </c>
       <c r="D170" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "luana.mourao" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C171" t="s">
         <v>1</v>
       </c>
       <c r="D171" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "mariana.brider" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C172" t="s">
         <v>1</v>
       </c>
       <c r="D172" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "adriana.paes" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C173" t="s">
         <v>1</v>
       </c>
       <c r="D173" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "larissa.rocha" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C174" t="s">
         <v>1</v>
       </c>
       <c r="D174" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "livia.hallack" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>85</v>
@@ -5799,142 +5754,142 @@
       </c>
       <c r="D175" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "vanessa.cirilo" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C176" t="s">
         <v>1</v>
       </c>
       <c r="D176" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "milena.ribeiral" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C177" t="s">
         <v>1</v>
       </c>
       <c r="D177" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "tatiane.neto" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C178" t="s">
         <v>1</v>
       </c>
       <c r="D178" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "tatyene.nehrer" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C179" t="s">
         <v>1</v>
       </c>
       <c r="D179" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "victor.quinet" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C180" t="s">
         <v>1</v>
       </c>
       <c r="D180" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "lidice.lenz" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C181" t="s">
         <v>1</v>
       </c>
       <c r="D181" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "alberlania.muller" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C182" t="s">
         <v>1</v>
       </c>
       <c r="D182" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "marcia.costa" ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C183" t="s">
         <v>1</v>
       </c>
       <c r="D183" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO vanessa ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C184" t="s">
         <v>1</v>
       </c>
       <c r="D184" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO aline ;</v>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "alice.gomes" ;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Criação da tela de autorização para finaliza_tratamento.php
</commit_message>
<xml_diff>
--- a/script_base_dados/grants_solus.xlsx
+++ b/script_base_dados/grants_solus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\solus\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57956E22-DAF9-45F7-9C94-4C5B8937B0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E8EDB5-3E5A-43D0-A336-86C664A24AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
   <sheets>
     <sheet name="grants" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="93">
   <si>
     <t>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO</t>
   </si>
@@ -293,6 +293,27 @@
   </si>
   <si>
     <t>"alice.gomes"</t>
+  </si>
+  <si>
+    <t>GRANT ALL ON SEQUENCE tratamento.sq_grupo_acesso TO</t>
+  </si>
+  <si>
+    <t>GRANT ALL ON SEQUENCE tratamento.sq_hstr_pnel_solic_trtmto TO</t>
+  </si>
+  <si>
+    <t>GRANT ALL ON SEQUENCE tratamento.sq_local_trtmto TO</t>
+  </si>
+  <si>
+    <t>GRANT ALL ON SEQUENCE tratamento.sq_risco_pcnt TO</t>
+  </si>
+  <si>
+    <t>GRANT ALL ON SEQUENCE tratamento.sq_status_pcnt TO</t>
+  </si>
+  <si>
+    <t>GRANT ALL ON SEQUENCE tratamento.sq_status_trtmto TO</t>
+  </si>
+  <si>
+    <t>"mariana.brider"</t>
   </si>
 </sst>
 </file>
@@ -3120,9 +3141,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F5A992-25FF-475C-9CF2-7DC64A66C30C}">
-  <dimension ref="A1:D184"/>
+  <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D185" sqref="D185:D206"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5078,7 +5101,7 @@
         <v>1</v>
       </c>
       <c r="D130" t="str">
-        <f t="shared" ref="D130:D184" si="2">A130&amp;" "&amp;B130&amp;" "&amp;C130</f>
+        <f t="shared" ref="D130:D193" si="2">A130&amp;" "&amp;B130&amp;" "&amp;C130</f>
         <v>GRANT DELETE, INSERT, SELECT, UPDATE ON TABLE tratamento.tb_c_cnvo TO "alice.gomes" ;</v>
       </c>
     </row>
@@ -5890,6 +5913,336 @@
       <c r="D184" t="str">
         <f t="shared" si="2"/>
         <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "alice.gomes" ;</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>55</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C185" t="s">
+        <v>1</v>
+      </c>
+      <c r="D185" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_acesso_transac_tratamento TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>82</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C186" t="s">
+        <v>1</v>
+      </c>
+      <c r="D186" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_cnvo TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>61</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C187" t="s">
+        <v>1</v>
+      </c>
+      <c r="D187" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>84</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C188" t="s">
+        <v>1</v>
+      </c>
+      <c r="D188" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_equipe_usua TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>86</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C189" t="s">
+        <v>1</v>
+      </c>
+      <c r="D189" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_acesso TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>56</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C190" t="s">
+        <v>1</v>
+      </c>
+      <c r="D190" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_usua_acesso TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>57</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C191" t="s">
+        <v>1</v>
+      </c>
+      <c r="D191" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_usua_menu_sist_tratamento TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>58</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C192" t="s">
+        <v>1</v>
+      </c>
+      <c r="D192" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_grupo_usua_transac_acesso TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>73</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C193" t="s">
+        <v>1</v>
+      </c>
+      <c r="D193" t="str">
+        <f t="shared" si="2"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_obs_pnel_mapa_risco TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>70</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C194" t="s">
+        <v>1</v>
+      </c>
+      <c r="D194" t="str">
+        <f t="shared" ref="D194:D206" si="3">A194&amp;" "&amp;B194&amp;" "&amp;C194</f>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_obs_pnel_solic_trtmto TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>72</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C195" t="s">
+        <v>1</v>
+      </c>
+      <c r="D195" t="str">
+        <f t="shared" si="3"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_pnel_mapa_risco TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>87</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C196" t="s">
+        <v>1</v>
+      </c>
+      <c r="D196" t="str">
+        <f t="shared" si="3"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_hstr_pnel_solic_trtmto TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>88</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C197" t="s">
+        <v>1</v>
+      </c>
+      <c r="D197" t="str">
+        <f t="shared" si="3"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_local_trtmto TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>54</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C198" t="s">
+        <v>1</v>
+      </c>
+      <c r="D198" t="str">
+        <f t="shared" si="3"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_log_acesso TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>59</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C199" t="s">
+        <v>1</v>
+      </c>
+      <c r="D199" t="str">
+        <f t="shared" si="3"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_menu_sist_tratamento TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>79</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C200" t="s">
+        <v>1</v>
+      </c>
+      <c r="D200" t="str">
+        <f t="shared" si="3"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pddo_trtmto TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>62</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C201" t="s">
+        <v>1</v>
+      </c>
+      <c r="D201" t="str">
+        <f t="shared" si="3"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_pnel_solic_trtmto TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>89</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C202" t="s">
+        <v>1</v>
+      </c>
+      <c r="D202" t="str">
+        <f t="shared" si="3"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_risco_pcnt TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>71</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C203" t="s">
+        <v>1</v>
+      </c>
+      <c r="D203" t="str">
+        <f t="shared" si="3"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_risco_rnado_pcnt TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>90</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C204" t="s">
+        <v>1</v>
+      </c>
+      <c r="D204" t="str">
+        <f t="shared" si="3"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_status_pcnt TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>91</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C205" t="s">
+        <v>1</v>
+      </c>
+      <c r="D205" t="str">
+        <f t="shared" si="3"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_status_trtmto TO "mariana.brider" ;</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>60</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C206" t="s">
+        <v>1</v>
+      </c>
+      <c r="D206" t="str">
+        <f t="shared" si="3"/>
+        <v>GRANT ALL ON SEQUENCE tratamento.sq_usua_acesso TO "mariana.brider" ;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>